<commit_message>
split part of all table
</commit_message>
<xml_diff>
--- a/i01py_excel/example1.xlsx
+++ b/i01py_excel/example1.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abel/Downloads/AbelProject/PythonProjectLearn/i01py_excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B1E5A24-A9FF-F44A-940D-7E9FFED15454}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{642047D5-EF22-0249-BD5B-F05C8E156172}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16060" activeTab="2" xr2:uid="{2EDB97D1-630C-5B4E-900C-92C25FCEBF35}"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="28240" windowHeight="16060" activeTab="4" xr2:uid="{2EDB97D1-630C-5B4E-900C-92C25FCEBF35}"/>
   </bookViews>
   <sheets>
     <sheet name="新工作表" sheetId="2" r:id="rId1"/>
-    <sheet name="SheetNew1" sheetId="1" r:id="rId2"/>
-    <sheet name="SheetNew2" sheetId="3" r:id="rId3"/>
+    <sheet name="SheetNewNew1" sheetId="1" r:id="rId2"/>
+    <sheet name="SheetNewNew2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -475,7 +477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC072628-6E07-4A4F-9CAA-8C6DA2A5D6C5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -490,4 +492,30 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34003258-ED3B-E14B-88A5-C66481F22DD9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24CD0E50-D664-2240-ADCB-76882EA57498}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>